<commit_message>
Implementation of new particulate matter model + update of the plastic model + corrections in ei mappings.
</commit_message>
<xml_diff>
--- a/Data/mappings/exiobase/EXIO_IW_concordance.xlsx
+++ b/Data/mappings/exiobase/EXIO_IW_concordance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings_2.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\exiobase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688DAE3E-B60E-4950-BB9B-474D7CD56935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886DB076-5809-4E2D-BAE5-53F0B4C45618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="1179">
   <si>
     <t>Taxes less subsidies on products purchased: Total</t>
   </si>
@@ -3597,6 +3597,9 @@
   </si>
   <si>
     <t>Occupation, unspecified</t>
+  </si>
+  <si>
+    <t>Pelagic fish</t>
   </si>
 </sst>
 </file>
@@ -3966,7 +3969,7 @@
   <dimension ref="A1:B1114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7683,11 +7686,17 @@
       <c r="A476" s="2" t="s">
         <v>471</v>
       </c>
+      <c r="B476" t="s">
+        <v>1178</v>
+      </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" s="2" t="s">
         <v>472</v>
       </c>
+      <c r="B477" t="s">
+        <v>1178</v>
+      </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" s="2" t="s">
@@ -9619,82 +9628,88 @@
         <v>843</v>
       </c>
     </row>
-    <row r="849" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="849" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A849" s="2" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="850" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="850" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A850" s="2" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="851" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="851" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A851" s="2" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="852" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="852" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A852" s="2" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="853" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="853" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A853" s="2" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="854" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="854" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A854" s="2" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="855" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="855" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A855" s="2" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="856" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="856" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A856" s="2" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="857" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B856" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A857" s="2" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="858" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B857" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A858" s="2" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="859" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="859" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A859" s="2" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="860" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="860" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A860" s="2" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="861" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="861" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A861" s="2" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="862" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="862" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A862" s="2" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="863" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="863" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A863" s="2" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="864" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="864" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A864" s="2" t="s">
         <v>859</v>
       </c>

</xml_diff>

<commit_message>
Minor corrections + final release for 2.1 version
</commit_message>
<xml_diff>
--- a/Data/mappings/exiobase/EXIO_IW_concordance.xlsx
+++ b/Data/mappings/exiobase/EXIO_IW_concordance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\exiobase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7032E0B6-E4BE-4A4E-B5C4-A8FDE15637CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B0619E-782A-4ED7-B1E7-6A475499CE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3527,12 +3527,6 @@
     <t>Perlite</t>
   </si>
   <si>
-    <t>Water, agri</t>
-  </si>
-  <si>
-    <t>Water, non-agri</t>
-  </si>
-  <si>
     <t>Iron</t>
   </si>
   <si>
@@ -3609,6 +3603,12 @@
   </si>
   <si>
     <t>Carbon dioxide, biogenic, release</t>
+  </si>
+  <si>
+    <t>Water, cooling, unspecified natural origin</t>
+  </si>
+  <si>
+    <t>Water, unspecified natural origin</t>
   </si>
 </sst>
 </file>
@@ -3977,7 +3977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4005,17 +4007,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4257,7 +4259,7 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -4265,7 +4267,7 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -4273,7 +4275,7 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -4281,7 +4283,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -4289,7 +4291,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -4297,7 +4299,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -4305,7 +4307,7 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -4313,7 +4315,7 @@
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -4321,7 +4323,7 @@
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -4329,7 +4331,7 @@
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -4337,7 +4339,7 @@
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -4345,7 +4347,7 @@
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -4353,7 +4355,7 @@
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -4361,7 +4363,7 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -4369,7 +4371,7 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -4377,7 +4379,7 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -4385,7 +4387,7 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -4681,7 +4683,7 @@
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -4689,7 +4691,7 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -4697,7 +4699,7 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -4705,7 +4707,7 @@
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -4713,7 +4715,7 @@
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -4721,7 +4723,7 @@
         <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -4729,7 +4731,7 @@
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -4737,7 +4739,7 @@
         <v>98</v>
       </c>
       <c r="B103" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -4745,7 +4747,7 @@
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -4753,7 +4755,7 @@
         <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -4761,7 +4763,7 @@
         <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -4769,7 +4771,7 @@
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -4777,7 +4779,7 @@
         <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -4785,7 +4787,7 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -4793,7 +4795,7 @@
         <v>105</v>
       </c>
       <c r="B110" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -4801,7 +4803,7 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -4809,7 +4811,7 @@
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -4817,7 +4819,7 @@
         <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -4825,7 +4827,7 @@
         <v>109</v>
       </c>
       <c r="B114" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -4833,7 +4835,7 @@
         <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -4841,7 +4843,7 @@
         <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -4849,7 +4851,7 @@
         <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -4857,7 +4859,7 @@
         <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -4865,7 +4867,7 @@
         <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -4873,7 +4875,7 @@
         <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -4881,7 +4883,7 @@
         <v>116</v>
       </c>
       <c r="B121" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -4889,7 +4891,7 @@
         <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -4913,7 +4915,7 @@
         <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -4921,7 +4923,7 @@
         <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -4929,7 +4931,7 @@
         <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -4937,7 +4939,7 @@
         <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -4945,7 +4947,7 @@
         <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -4953,7 +4955,7 @@
         <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -4961,7 +4963,7 @@
         <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -4969,7 +4971,7 @@
         <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -4977,7 +4979,7 @@
         <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -4993,7 +4995,7 @@
         <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -5001,7 +5003,7 @@
         <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -5009,7 +5011,7 @@
         <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -5017,7 +5019,7 @@
         <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -5609,7 +5611,7 @@
         <v>207</v>
       </c>
       <c r="B212" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -5617,7 +5619,7 @@
         <v>208</v>
       </c>
       <c r="B213" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -5625,7 +5627,7 @@
         <v>209</v>
       </c>
       <c r="B214" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
@@ -5633,7 +5635,7 @@
         <v>210</v>
       </c>
       <c r="B215" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -5641,7 +5643,7 @@
         <v>211</v>
       </c>
       <c r="B216" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -5649,7 +5651,7 @@
         <v>212</v>
       </c>
       <c r="B217" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -5657,7 +5659,7 @@
         <v>213</v>
       </c>
       <c r="B218" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -5665,7 +5667,7 @@
         <v>214</v>
       </c>
       <c r="B219" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -6553,7 +6555,7 @@
         <v>325</v>
       </c>
       <c r="B330" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -6561,7 +6563,7 @@
         <v>326</v>
       </c>
       <c r="B331" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -6569,7 +6571,7 @@
         <v>327</v>
       </c>
       <c r="B332" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -6577,7 +6579,7 @@
         <v>328</v>
       </c>
       <c r="B333" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -6585,7 +6587,7 @@
         <v>329</v>
       </c>
       <c r="B334" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -6593,7 +6595,7 @@
         <v>330</v>
       </c>
       <c r="B335" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -6601,7 +6603,7 @@
         <v>331</v>
       </c>
       <c r="B336" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -6609,7 +6611,7 @@
         <v>332</v>
       </c>
       <c r="B337" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
@@ -6617,7 +6619,7 @@
         <v>333</v>
       </c>
       <c r="B338" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -6625,7 +6627,7 @@
         <v>334</v>
       </c>
       <c r="B339" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
@@ -6633,7 +6635,7 @@
         <v>335</v>
       </c>
       <c r="B340" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -6641,7 +6643,7 @@
         <v>336</v>
       </c>
       <c r="B341" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
@@ -6649,7 +6651,7 @@
         <v>337</v>
       </c>
       <c r="B342" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -6657,7 +6659,7 @@
         <v>338</v>
       </c>
       <c r="B343" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -6817,7 +6819,7 @@
         <v>358</v>
       </c>
       <c r="B363" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
@@ -6825,7 +6827,7 @@
         <v>359</v>
       </c>
       <c r="B364" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
@@ -6833,7 +6835,7 @@
         <v>360</v>
       </c>
       <c r="B365" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
@@ -6841,7 +6843,7 @@
         <v>361</v>
       </c>
       <c r="B366" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
@@ -7217,7 +7219,7 @@
         <v>408</v>
       </c>
       <c r="B413" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
@@ -7225,7 +7227,7 @@
         <v>409</v>
       </c>
       <c r="B414" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
@@ -7233,7 +7235,7 @@
         <v>410</v>
       </c>
       <c r="B415" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
@@ -7241,7 +7243,7 @@
         <v>411</v>
       </c>
       <c r="B416" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
@@ -7249,7 +7251,7 @@
         <v>412</v>
       </c>
       <c r="B417" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
@@ -7257,7 +7259,7 @@
         <v>413</v>
       </c>
       <c r="B418" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
@@ -7265,7 +7267,7 @@
         <v>414</v>
       </c>
       <c r="B419" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
@@ -7273,7 +7275,7 @@
         <v>415</v>
       </c>
       <c r="B420" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
@@ -7281,7 +7283,7 @@
         <v>416</v>
       </c>
       <c r="B421" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
@@ -7289,7 +7291,7 @@
         <v>417</v>
       </c>
       <c r="B422" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
@@ -7297,7 +7299,7 @@
         <v>418</v>
       </c>
       <c r="B423" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
@@ -7305,7 +7307,7 @@
         <v>419</v>
       </c>
       <c r="B424" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
@@ -7422,7 +7424,7 @@
         <v>434</v>
       </c>
       <c r="B439" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
@@ -7603,7 +7605,7 @@
         <v>457</v>
       </c>
       <c r="B462" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
@@ -7694,7 +7696,7 @@
         <v>471</v>
       </c>
       <c r="B476" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
@@ -7702,7 +7704,7 @@
         <v>472</v>
       </c>
       <c r="B477" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
@@ -7874,7 +7876,7 @@
         <v>501</v>
       </c>
       <c r="B506" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
@@ -7898,7 +7900,7 @@
         <v>504</v>
       </c>
       <c r="B509" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.3">
@@ -9675,7 +9677,7 @@
         <v>851</v>
       </c>
       <c r="B856" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.3">
@@ -9683,7 +9685,7 @@
         <v>852</v>
       </c>
       <c r="B857" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.3">
@@ -9919,7 +9921,7 @@
         <v>889</v>
       </c>
       <c r="B894" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.3">
@@ -9943,7 +9945,7 @@
         <v>892</v>
       </c>
       <c r="B897" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.3">
@@ -10125,7 +10127,7 @@
         <v>920</v>
       </c>
       <c r="B925" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.3">
@@ -10133,7 +10135,7 @@
         <v>921</v>
       </c>
       <c r="B926" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.3">
@@ -10141,7 +10143,7 @@
         <v>922</v>
       </c>
       <c r="B927" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.3">
@@ -10149,7 +10151,7 @@
         <v>923</v>
       </c>
       <c r="B928" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.3">
@@ -10157,7 +10159,7 @@
         <v>924</v>
       </c>
       <c r="B929" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.3">
@@ -10165,7 +10167,7 @@
         <v>925</v>
       </c>
       <c r="B930" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.3">
@@ -10173,7 +10175,7 @@
         <v>926</v>
       </c>
       <c r="B931" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.3">
@@ -10181,7 +10183,7 @@
         <v>927</v>
       </c>
       <c r="B932" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.3">
@@ -10189,7 +10191,7 @@
         <v>928</v>
       </c>
       <c r="B933" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.3">
@@ -10197,7 +10199,7 @@
         <v>929</v>
       </c>
       <c r="B934" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.3">
@@ -10205,7 +10207,7 @@
         <v>930</v>
       </c>
       <c r="B935" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.3">
@@ -10213,7 +10215,7 @@
         <v>931</v>
       </c>
       <c r="B936" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.3">
@@ -10221,7 +10223,7 @@
         <v>932</v>
       </c>
       <c r="B937" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.3">
@@ -10229,7 +10231,7 @@
         <v>933</v>
       </c>
       <c r="B938" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.3">
@@ -10237,7 +10239,7 @@
         <v>934</v>
       </c>
       <c r="B939" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.3">
@@ -10245,7 +10247,7 @@
         <v>935</v>
       </c>
       <c r="B940" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.3">
@@ -10253,7 +10255,7 @@
         <v>936</v>
       </c>
       <c r="B941" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.3">
@@ -10261,7 +10263,7 @@
         <v>937</v>
       </c>
       <c r="B942" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.3">
@@ -10269,7 +10271,7 @@
         <v>938</v>
       </c>
       <c r="B943" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.3">
@@ -10277,7 +10279,7 @@
         <v>939</v>
       </c>
       <c r="B944" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.3">
@@ -10285,7 +10287,7 @@
         <v>940</v>
       </c>
       <c r="B945" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.3">
@@ -10293,7 +10295,7 @@
         <v>941</v>
       </c>
       <c r="B946" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.3">
@@ -10301,7 +10303,7 @@
         <v>942</v>
       </c>
       <c r="B947" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.3">
@@ -10309,7 +10311,7 @@
         <v>943</v>
       </c>
       <c r="B948" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.3">
@@ -10317,7 +10319,7 @@
         <v>944</v>
       </c>
       <c r="B949" t="s">
-        <v>1154</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.3">
@@ -10325,7 +10327,7 @@
         <v>945</v>
       </c>
       <c r="B950" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.3">
@@ -10333,7 +10335,7 @@
         <v>946</v>
       </c>
       <c r="B951" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.3">
@@ -10341,7 +10343,7 @@
         <v>947</v>
       </c>
       <c r="B952" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.3">
@@ -10349,7 +10351,7 @@
         <v>948</v>
       </c>
       <c r="B953" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.3">
@@ -10357,7 +10359,7 @@
         <v>949</v>
       </c>
       <c r="B954" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.3">
@@ -10365,7 +10367,7 @@
         <v>950</v>
       </c>
       <c r="B955" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.3">
@@ -10373,7 +10375,7 @@
         <v>951</v>
       </c>
       <c r="B956" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.3">
@@ -10381,7 +10383,7 @@
         <v>952</v>
       </c>
       <c r="B957" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.3">
@@ -10389,7 +10391,7 @@
         <v>953</v>
       </c>
       <c r="B958" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.3">
@@ -10397,7 +10399,7 @@
         <v>954</v>
       </c>
       <c r="B959" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.3">
@@ -10405,7 +10407,7 @@
         <v>955</v>
       </c>
       <c r="B960" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.3">
@@ -10413,7 +10415,7 @@
         <v>956</v>
       </c>
       <c r="B961" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.3">
@@ -10421,7 +10423,7 @@
         <v>957</v>
       </c>
       <c r="B962" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.3">
@@ -10429,7 +10431,7 @@
         <v>958</v>
       </c>
       <c r="B963" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.3">
@@ -10437,7 +10439,7 @@
         <v>959</v>
       </c>
       <c r="B964" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.3">
@@ -10445,7 +10447,7 @@
         <v>960</v>
       </c>
       <c r="B965" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.3">
@@ -10453,7 +10455,7 @@
         <v>961</v>
       </c>
       <c r="B966" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.3">
@@ -10461,7 +10463,7 @@
         <v>962</v>
       </c>
       <c r="B967" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.3">
@@ -10469,7 +10471,7 @@
         <v>963</v>
       </c>
       <c r="B968" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.3">
@@ -10477,7 +10479,7 @@
         <v>964</v>
       </c>
       <c r="B969" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.3">
@@ -10485,7 +10487,7 @@
         <v>965</v>
       </c>
       <c r="B970" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.3">
@@ -10493,7 +10495,7 @@
         <v>966</v>
       </c>
       <c r="B971" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.3">
@@ -10501,7 +10503,7 @@
         <v>967</v>
       </c>
       <c r="B972" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.3">
@@ -10509,7 +10511,7 @@
         <v>968</v>
       </c>
       <c r="B973" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.3">
@@ -10517,7 +10519,7 @@
         <v>969</v>
       </c>
       <c r="B974" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.3">
@@ -10525,7 +10527,7 @@
         <v>970</v>
       </c>
       <c r="B975" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.3">
@@ -10533,7 +10535,7 @@
         <v>971</v>
       </c>
       <c r="B976" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.3">
@@ -10541,7 +10543,7 @@
         <v>972</v>
       </c>
       <c r="B977" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.3">
@@ -10549,7 +10551,7 @@
         <v>973</v>
       </c>
       <c r="B978" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.3">
@@ -10557,7 +10559,7 @@
         <v>974</v>
       </c>
       <c r="B979" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.3">
@@ -10565,7 +10567,7 @@
         <v>975</v>
       </c>
       <c r="B980" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.3">
@@ -10573,7 +10575,7 @@
         <v>976</v>
       </c>
       <c r="B981" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.3">
@@ -10581,7 +10583,7 @@
         <v>977</v>
       </c>
       <c r="B982" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.3">
@@ -10589,7 +10591,7 @@
         <v>978</v>
       </c>
       <c r="B983" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.3">
@@ -10597,7 +10599,7 @@
         <v>979</v>
       </c>
       <c r="B984" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.3">
@@ -10605,7 +10607,7 @@
         <v>980</v>
       </c>
       <c r="B985" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.3">
@@ -10613,7 +10615,7 @@
         <v>981</v>
       </c>
       <c r="B986" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.3">
@@ -10621,7 +10623,7 @@
         <v>982</v>
       </c>
       <c r="B987" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.3">
@@ -10629,7 +10631,7 @@
         <v>983</v>
       </c>
       <c r="B988" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.3">
@@ -10637,7 +10639,7 @@
         <v>984</v>
       </c>
       <c r="B989" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.3">
@@ -10645,7 +10647,7 @@
         <v>985</v>
       </c>
       <c r="B990" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.3">
@@ -10653,7 +10655,7 @@
         <v>986</v>
       </c>
       <c r="B991" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.3">
@@ -10661,7 +10663,7 @@
         <v>987</v>
       </c>
       <c r="B992" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.3">
@@ -10669,7 +10671,7 @@
         <v>988</v>
       </c>
       <c r="B993" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.3">
@@ -10677,7 +10679,7 @@
         <v>989</v>
       </c>
       <c r="B994" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.3">
@@ -10685,7 +10687,7 @@
         <v>990</v>
       </c>
       <c r="B995" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.3">
@@ -10693,7 +10695,7 @@
         <v>991</v>
       </c>
       <c r="B996" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.3">
@@ -10701,7 +10703,7 @@
         <v>992</v>
       </c>
       <c r="B997" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.3">
@@ -10709,7 +10711,7 @@
         <v>993</v>
       </c>
       <c r="B998" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.3">
@@ -10717,7 +10719,7 @@
         <v>994</v>
       </c>
       <c r="B999" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.3">
@@ -10725,7 +10727,7 @@
         <v>995</v>
       </c>
       <c r="B1000" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.3">
@@ -10733,7 +10735,7 @@
         <v>996</v>
       </c>
       <c r="B1001" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.3">
@@ -10741,7 +10743,7 @@
         <v>997</v>
       </c>
       <c r="B1002" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.3">
@@ -10749,7 +10751,7 @@
         <v>998</v>
       </c>
       <c r="B1003" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.3">
@@ -10757,7 +10759,7 @@
         <v>999</v>
       </c>
       <c r="B1004" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.3">
@@ -10765,7 +10767,7 @@
         <v>1000</v>
       </c>
       <c r="B1005" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.3">
@@ -10773,7 +10775,7 @@
         <v>1001</v>
       </c>
       <c r="B1006" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.3">
@@ -10781,7 +10783,7 @@
         <v>1002</v>
       </c>
       <c r="B1007" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.3">
@@ -10789,7 +10791,7 @@
         <v>1003</v>
       </c>
       <c r="B1008" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.3">
@@ -10797,7 +10799,7 @@
         <v>1004</v>
       </c>
       <c r="B1009" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.3">
@@ -10805,7 +10807,7 @@
         <v>1005</v>
       </c>
       <c r="B1010" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.3">
@@ -10813,7 +10815,7 @@
         <v>1006</v>
       </c>
       <c r="B1011" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.3">
@@ -10821,7 +10823,7 @@
         <v>1007</v>
       </c>
       <c r="B1012" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.3">
@@ -10829,7 +10831,7 @@
         <v>1008</v>
       </c>
       <c r="B1013" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.3">
@@ -10837,7 +10839,7 @@
         <v>1009</v>
       </c>
       <c r="B1014" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.3">
@@ -10845,7 +10847,7 @@
         <v>1010</v>
       </c>
       <c r="B1015" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.3">
@@ -10853,7 +10855,7 @@
         <v>1011</v>
       </c>
       <c r="B1016" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.3">
@@ -10861,7 +10863,7 @@
         <v>1012</v>
       </c>
       <c r="B1017" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.3">
@@ -10869,7 +10871,7 @@
         <v>1013</v>
       </c>
       <c r="B1018" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.3">
@@ -10877,7 +10879,7 @@
         <v>1014</v>
       </c>
       <c r="B1019" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.3">
@@ -10885,7 +10887,7 @@
         <v>1015</v>
       </c>
       <c r="B1020" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.3">
@@ -10893,7 +10895,7 @@
         <v>1016</v>
       </c>
       <c r="B1021" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.3">
@@ -10901,7 +10903,7 @@
         <v>1017</v>
       </c>
       <c r="B1022" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.3">
@@ -10909,7 +10911,7 @@
         <v>1018</v>
       </c>
       <c r="B1023" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.3">
@@ -10917,7 +10919,7 @@
         <v>1019</v>
       </c>
       <c r="B1024" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.3">
@@ -10925,7 +10927,7 @@
         <v>1020</v>
       </c>
       <c r="B1025" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.3">
@@ -10933,7 +10935,7 @@
         <v>1021</v>
       </c>
       <c r="B1026" t="s">
-        <v>1155</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.3">
@@ -10941,7 +10943,7 @@
         <v>1022</v>
       </c>
       <c r="B1027" t="s">
-        <v>1155</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.3">
@@ -11336,47 +11338,47 @@
     </row>
     <row r="1106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1106" s="2" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1107" s="2" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1108" s="2" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1109" s="2" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1110" s="2" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1111" s="2" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1112" s="2" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1113" s="2" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1114" s="2" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>